<commit_message>
Modifying the Carnet de bord structure
</commit_message>
<xml_diff>
--- a/lib/files/Carnet_de_bord.xlsx
+++ b/lib/files/Carnet_de_bord.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8511125A-B004-4D9A-9E97-5CE6150DD8B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DDFCF3-C292-4FA0-93BA-C93C17623206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -74,13 +74,37 @@
   </si>
   <si>
     <t>12345678910</t>
+  </si>
+  <si>
+    <t>Type du véhicule</t>
+  </si>
+  <si>
+    <t>Marque du véhicule</t>
+  </si>
+  <si>
+    <t>Modèle du véhicule</t>
+  </si>
+  <si>
+    <t>Voiture</t>
+  </si>
+  <si>
+    <t>Mercedes</t>
+  </si>
+  <si>
+    <t>Classe G63 AMG 544ch</t>
+  </si>
+  <si>
+    <t>Id de l'unité</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +125,14 @@
       <color indexed="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -157,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -171,9 +203,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -181,6 +210,11 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,93 +553,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02F03FD0-1C6C-43E9-91A0-04D7513DFAC3}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.44140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
-    <col min="8" max="8" width="2.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
-    <col min="11" max="11" width="8" customWidth="1"/>
-    <col min="12" max="12" width="14.5546875" customWidth="1"/>
+    <col min="1" max="6" width="11.44140625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="30.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="2.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" customWidth="1"/>
+    <col min="15" max="15" width="8" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5">
+      <c r="J2" s="8">
         <v>5</v>
       </c>
-      <c r="G2" s="5">
+      <c r="K2" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F3">
+      <c r="J3" s="10">
         <v>10</v>
       </c>
-      <c r="G3">
+      <c r="K3" s="10">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementing the file upload on server side for the planning generation
</commit_message>
<xml_diff>
--- a/lib/files/Carnet_de_bord.xlsx
+++ b/lib/files/Carnet_de_bord.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DDFCF3-C292-4FA0-93BA-C93C17623206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095CC54B-8DC8-4C25-BC2C-7672E1385D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="2364" windowWidth="18120" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Carnet de bord" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -46,27 +46,6 @@
     <t xml:space="preserve">Compteur à la fin du déplacement </t>
   </si>
   <si>
-    <t>descriptif test</t>
-  </si>
-  <si>
-    <t>nom test</t>
-  </si>
-  <si>
-    <t>personne test</t>
-  </si>
-  <si>
-    <t>deuxieme descriptif test</t>
-  </si>
-  <si>
-    <t>deuxieme nom test</t>
-  </si>
-  <si>
-    <t>deuxieme personne test</t>
-  </si>
-  <si>
-    <t>2020-06-25</t>
-  </si>
-  <si>
     <t>2020-06-26</t>
   </si>
   <si>
@@ -98,13 +77,52 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Repérage</t>
+  </si>
+  <si>
+    <t>Mohamed Amine BENBAKHTA</t>
+  </si>
+  <si>
+    <t>Lotfi Rdjem DARSOUNI</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2020-06-27</t>
+  </si>
+  <si>
+    <t>2020-06-28</t>
+  </si>
+  <si>
+    <t>2020-06-29</t>
+  </si>
+  <si>
+    <t>Livraison</t>
+  </si>
+  <si>
+    <t>Mission</t>
+  </si>
+  <si>
+    <t>Retour Mission</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,12 +145,24 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -189,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -200,21 +230,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,15 +586,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02F03FD0-1C6C-43E9-91A0-04D7513DFAC3}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="11.44140625" style="7" customWidth="1"/>
+    <col min="1" max="6" width="11.44140625" style="5" customWidth="1"/>
     <col min="7" max="7" width="30.44140625" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" customWidth="1"/>
     <col min="9" max="9" width="12.88671875" customWidth="1"/>
@@ -575,23 +608,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>18</v>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
@@ -610,76 +643,217 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="E2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="8">
+        <v>100</v>
+      </c>
+      <c r="K2" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="10">
+        <v>200</v>
+      </c>
+      <c r="K3" s="10">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="10">
+        <v>350</v>
+      </c>
+      <c r="K4" s="10">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="10">
+        <v>450</v>
+      </c>
+      <c r="K5" s="10">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="10">
+        <v>700</v>
+      </c>
+      <c r="K6" s="10">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="8">
-        <v>5</v>
-      </c>
-      <c r="K2" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="10">
-        <v>10</v>
-      </c>
-      <c r="K3" s="10">
-        <v>15</v>
+      <c r="I7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="10">
+        <v>950</v>
+      </c>
+      <c r="K7" s="10">
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.27559055118110237" right="0.31496062992125984" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>

</xml_diff>